<commit_message>
Testing util for data table
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/DecisionTreeLearnerTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/DecisionTreeLearnerTest.xlsx
@@ -13,14 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="golf" sheetId="1" r:id="rId1"/>
-    <sheet name="Definition" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
   <si>
     <t>Outlook</t>
   </si>
@@ -55,13 +54,19 @@
     <t>#0</t>
   </si>
   <si>
-    <t>golf[outlook]</t>
+    <t>typedef</t>
   </si>
   <si>
-    <t>golf[wind]</t>
+    <t>Boolean</t>
   </si>
   <si>
-    <t>golf[play]</t>
+    <t>YesOrNo</t>
+  </si>
+  <si>
+    <t>column-def</t>
+  </si>
+  <si>
+    <t>#1</t>
   </si>
 </sst>
 </file>
@@ -851,112 +856,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A2:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:E32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>85</v>
-      </c>
-      <c r="C2">
-        <v>85</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>80</v>
-      </c>
-      <c r="C3">
-        <v>90</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C4">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C5">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="C6">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -970,30 +959,30 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C7">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C8">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -1001,16 +990,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C9">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -1018,16 +1007,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C10">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -1035,19 +1024,19 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C11">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1055,13 +1044,13 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C12">
         <v>70</v>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -1069,16 +1058,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C13">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1086,16 +1075,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C14">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1103,415 +1092,531 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C15">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>81</v>
+      </c>
+      <c r="C16">
+        <v>75</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>71</v>
+      </c>
+      <c r="C17">
+        <v>80</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>14</v>
-      </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <f>VLOOKUP(A2,Definition!$A$2:$B$4,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="B19">
-        <f>B2</f>
-        <v>85</v>
-      </c>
-      <c r="C19">
-        <f>C2</f>
-        <v>85</v>
-      </c>
-      <c r="D19">
-        <f>IF(D2,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <f>VLOOKUP(E2,Definition!$A$10:$B$11,2,FALSE)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f>VLOOKUP(A3,Definition!$A$2:$B$4,2,FALSE)</f>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B20">
-        <f t="shared" ref="B20:C20" si="0">B3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f>VLOOKUP(A4,A$37:B$39,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <f>B4</f>
+        <v>85</v>
+      </c>
+      <c r="C21">
+        <f>C4</f>
+        <v>85</v>
+      </c>
+      <c r="D21">
+        <f>VLOOKUP(D4,A$42:B$43,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f>VLOOKUP(A5,A$37:B$39,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B22:C22" si="0">B5</f>
         <v>80</v>
       </c>
-      <c r="C20">
+      <c r="C22">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="D20">
-        <f t="shared" ref="D20:D32" si="1">IF(D3,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <f>VLOOKUP(E3,Definition!$A$10:$B$11,2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <f>VLOOKUP(A4,Definition!$A$2:$B$4,2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="B21">
-        <f t="shared" ref="B21:C21" si="2">B4</f>
-        <v>83</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="2"/>
-        <v>78</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <f>VLOOKUP(E4,Definition!$A$10:$B$11,2,FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <f>VLOOKUP(A5,Definition!$A$2:$B$4,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="B22">
-        <f t="shared" ref="B22:C22" si="3">B5</f>
-        <v>70</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="3"/>
-        <v>96</v>
-      </c>
       <c r="D22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <f>VLOOKUP(E5,Definition!$A$10:$B$11,2,FALSE)</f>
+        <f>VLOOKUP(D5,A$42:B$43,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f>VLOOKUP(A6,Definition!$A$2:$B$4,2,FALSE)</f>
-        <v>2</v>
+        <f>VLOOKUP(A6,A$37:B$39,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23:C23" si="4">B6</f>
-        <v>68</v>
+        <f t="shared" ref="B23:C23" si="1">B6</f>
+        <v>83</v>
       </c>
       <c r="C23">
-        <f t="shared" si="4"/>
-        <v>80</v>
+        <f t="shared" si="1"/>
+        <v>78</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <f>VLOOKUP(E6,Definition!$A$10:$B$11,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(D6,A$42:B$43,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <f>VLOOKUP(A7,Definition!$A$2:$B$4,2,FALSE)</f>
+        <f>VLOOKUP(A7,A$37:B$39,2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="B24">
-        <f t="shared" ref="B24:C24" si="5">B7</f>
-        <v>65</v>
+        <f t="shared" ref="B24:C24" si="2">B7</f>
+        <v>70</v>
       </c>
       <c r="C24">
-        <f t="shared" si="5"/>
-        <v>70</v>
+        <f t="shared" si="2"/>
+        <v>96</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <f>VLOOKUP(E7,Definition!$A$10:$B$11,2,FALSE)</f>
+        <f>VLOOKUP(D7,A$42:B$43,2,FALSE)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <f>VLOOKUP(A8,Definition!$A$2:$B$4,2,FALSE)</f>
-        <v>0</v>
+        <f>VLOOKUP(A8,A$37:B$39,2,FALSE)</f>
+        <v>2</v>
       </c>
       <c r="B25">
-        <f t="shared" ref="B25:C25" si="6">B8</f>
-        <v>64</v>
+        <f t="shared" ref="B25:C25" si="3">B8</f>
+        <v>68</v>
       </c>
       <c r="C25">
-        <f t="shared" si="6"/>
-        <v>65</v>
+        <f t="shared" si="3"/>
+        <v>80</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <f>VLOOKUP(E8,Definition!$A$10:$B$11,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(D8,A$42:B$43,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <f>VLOOKUP(A9,Definition!$A$2:$B$4,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(A9,A$37:B$39,2,FALSE)</f>
+        <v>2</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:C26" si="7">B9</f>
-        <v>72</v>
+        <f t="shared" ref="B26:C26" si="4">B9</f>
+        <v>65</v>
       </c>
       <c r="C26">
-        <f t="shared" si="7"/>
-        <v>95</v>
+        <f t="shared" si="4"/>
+        <v>70</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <f>VLOOKUP(E9,Definition!$A$10:$B$11,2,FALSE)</f>
-        <v>0</v>
+        <f>VLOOKUP(D9,A$42:B$43,2,FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <f>VLOOKUP(A10,Definition!$A$2:$B$4,2,FALSE)</f>
+        <f>VLOOKUP(A10,A$37:B$39,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="B27">
-        <f t="shared" ref="B27:C27" si="8">B10</f>
-        <v>69</v>
+        <f t="shared" ref="B27:C27" si="5">B10</f>
+        <v>64</v>
       </c>
       <c r="C27">
-        <f t="shared" si="8"/>
-        <v>70</v>
+        <f t="shared" si="5"/>
+        <v>65</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <f>VLOOKUP(E10,Definition!$A$10:$B$11,2,FALSE)</f>
+        <f>VLOOKUP(D10,A$42:B$43,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f>VLOOKUP(A11,Definition!$A$2:$B$4,2,FALSE)</f>
-        <v>2</v>
+        <f>VLOOKUP(A11,A$37:B$39,2,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28:C28" si="9">B11</f>
-        <v>75</v>
+        <f t="shared" ref="B28:C28" si="6">B11</f>
+        <v>72</v>
       </c>
       <c r="C28">
-        <f t="shared" si="9"/>
-        <v>80</v>
+        <f t="shared" si="6"/>
+        <v>95</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <f>VLOOKUP(E11,Definition!$A$10:$B$11,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(D11,A$42:B$43,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <f>VLOOKUP(A12,Definition!$A$2:$B$4,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(A12,A$37:B$39,2,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="B29">
-        <f t="shared" ref="B29:C29" si="10">B12</f>
-        <v>75</v>
+        <f t="shared" ref="B29:C29" si="7">B12</f>
+        <v>69</v>
       </c>
       <c r="C29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>70</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <f>VLOOKUP(E12,Definition!$A$10:$B$11,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(D12,A$42:B$43,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
-        <f>VLOOKUP(A13,Definition!$A$2:$B$4,2,FALSE)</f>
-        <v>0</v>
+        <f>VLOOKUP(A13,A$37:B$39,2,FALSE)</f>
+        <v>2</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30:C30" si="11">B13</f>
-        <v>72</v>
+        <f t="shared" ref="B30:C30" si="8">B13</f>
+        <v>75</v>
       </c>
       <c r="C30">
-        <f t="shared" si="11"/>
-        <v>90</v>
+        <f t="shared" si="8"/>
+        <v>80</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <f>VLOOKUP(E13,Definition!$A$10:$B$11,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(D13,A$42:B$43,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <f>VLOOKUP(A14,Definition!$A$2:$B$4,2,FALSE)</f>
+        <f>VLOOKUP(A14,A$37:B$39,2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="B31">
-        <f t="shared" ref="B31:C31" si="12">B14</f>
-        <v>81</v>
+        <f t="shared" ref="B31:C31" si="9">B14</f>
+        <v>75</v>
       </c>
       <c r="C31">
-        <f t="shared" si="12"/>
-        <v>75</v>
+        <f t="shared" si="9"/>
+        <v>70</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <f>VLOOKUP(E14,Definition!$A$10:$B$11,2,FALSE)</f>
+        <f>VLOOKUP(D14,A$42:B$43,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <f>VLOOKUP(A15,Definition!$A$2:$B$4,2,FALSE)</f>
+        <f>VLOOKUP(A15,A$37:B$39,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ref="B32:C32" si="10">B15</f>
+        <v>72</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="10"/>
+        <v>90</v>
+      </c>
+      <c r="D32">
+        <f>VLOOKUP(D15,A$42:B$43,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f>VLOOKUP(A16,A$37:B$39,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:C33" si="11">B16</f>
+        <v>81</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
+      <c r="D33">
+        <f>VLOOKUP(D16,A$42:B$43,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f>VLOOKUP(A17,A$37:B$39,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="B32">
-        <f t="shared" ref="B32:C32" si="13">B15</f>
+      <c r="B34">
+        <f t="shared" ref="B34:C34" si="12">B17</f>
         <v>71</v>
       </c>
-      <c r="C32">
+      <c r="C34">
+        <f t="shared" si="12"/>
+        <v>80</v>
+      </c>
+      <c r="D34">
+        <f>VLOOKUP(D17,A$42:B$43,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="b">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="b">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f>A20</f>
+        <v>14</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <f>VLOOKUP(E4,A$46:B$47,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <f t="shared" ref="A52:A64" si="13">VLOOKUP(E5,A$46:B$47,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
         <f t="shared" si="13"/>
-        <v>80</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <f>VLOOKUP(E15,Definition!$A$10:$B$11,2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <f>VLOOKUP(E14,A$46:B$47,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
+      <c r="C67" t="str">
+        <f>B41</f>
+        <v>Boolean</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68">
+        <v>-1</v>
+      </c>
+      <c r="C68" t="str">
+        <f>B45</f>
+        <v>YesOrNo</v>
       </c>
     </row>
   </sheetData>

</xml_diff>